<commit_message>
Analysis of patient metrics - mean and SD and comparison with ground truth
</commit_message>
<xml_diff>
--- a/Marching_Cubes/patient_metrics_marching_cubes.xlsx
+++ b/Marching_Cubes/patient_metrics_marching_cubes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/kaiwen_liu_mail_utoronto_ca/Documents/Desktop/github_repo/heart_cardiac_mri_image_processing/Marching_Cubes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_6E9D13ACD3005938B3F82A11595ED87656CD3863" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{306AAA4A-05D5-45A7-AA38-493F32663632}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_6E9D13ACD3005938B3F82A11595ED87656CD3863" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D619632-1E46-4ECD-B146-DE46CCEB64A2}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1425" yWindow="1425" windowWidth="26370" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="26370" windowHeight="13635" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,6 +353,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -642,12 +646,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" customWidth="1"/>

</xml_diff>